<commit_message>
Updated data processing and (hopefully) final network
</commit_message>
<xml_diff>
--- a/data/data_description.xlsx
+++ b/data/data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlous\Documents\Uni\Bayesian Networks\Assignment 1\heart-disease\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA048237-5D2E-4427-BB28-ADE77B0DD388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170D5B4D-51EB-4B11-A3B4-AEC9DC384E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1452" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>variable_name</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>[3, 6, 7]</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3]</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,7 +600,7 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>